<commit_message>
updates to part iii script and data entry and processing protocol
</commit_message>
<xml_diff>
--- a/data/digitized_data/HJ-7-occ-entry-template_22-11-29.xlsx
+++ b/data/digitized_data/HJ-7-occ-entry-template_22-11-29.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82264632-87B5-C745-A9A7-64F7649BE49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D640B96-49D6-3C48-8FE5-506DD243123A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -1358,7 +1358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" shapeId="0" xr:uid="{30FD4B1D-23D7-1145-B056-E0D6B319A5EB}">
+    <comment ref="O1" authorId="1" shapeId="0" xr:uid="{30FD4B1D-23D7-1145-B056-E0D6B319A5EB}">
       <text>
         <r>
           <rPr>
@@ -1444,7 +1444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" shapeId="0" xr:uid="{A2F25764-4BE8-0245-85D4-5F505ECE445E}">
+    <comment ref="P1" authorId="1" shapeId="0" xr:uid="{CA3A2C45-C583-DA43-877C-3A38B460B025}">
       <text>
         <r>
           <rPr>
@@ -1454,211 +1454,280 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">habitat 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Defintion: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>if habitat information provided, place here. This includes whether it is in an aquatic vs terrestrial habitat (aquatic, in lake shoreline), the biogeoclimatic zone, shading conditions (e.g. in shade, shaded, in sun) , relative position at locality (e.g. base vs seep vs ledge), position on habitat objects (e.g. on log)</t>
+          <t>vElev</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">verbatim elevation. The elevation in meters if provided
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Example</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">: 10 </t>
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1" shapeId="0" xr:uid="{CA3A2C45-C583-DA43-877C-3A38B460B025}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{9F8D95FB-54D3-F04C-9134-F2DD1CEAD6ED}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>vElev</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">verbatim elevation. The elevation in meters if provided
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Example</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">: 10 </t>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vLat 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Definition:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> verbatim latitude. The geographic latitude in decimal degrees or degrees minutes seconds. Positive values are north of the Equator, negative values are south of it. Legal values lie between -90 and 90, inclusive.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Examples: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> "-41.0983423". If degrees minutes seconds: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>49 39 12</t>
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1" shapeId="0" xr:uid="{2EA07FA5-5659-8C4C-AE40-A4B84A6793C3}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{A76DD89C-13AB-F048-A935-8FD1A912F16A}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">vElevReference
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Defintiion: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">verbatim elevation reference. Use this column if there were notes about how elevation was measured. </t>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">RECOMMENDED
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Definition:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">verbatim longitude. The geographic longitude in decimal degrees or degrees minutes seconds. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Positive values are east of the Greenwich Meridian, negative values are west of it. Legal values lie between -180 and 180, inclusive.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Examples: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> "-121.1761111". If in degrees minutes secons: 124 56 37</t>
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" shapeId="0" xr:uid="{B9586400-66D1-7141-8F4F-DF928AA236E2}">
+    <comment ref="S1" authorId="1" shapeId="0" xr:uid="{B3BFE285-5D7E-014B-96D5-A3177370E856}">
       <text>
         <r>
           <rPr>
@@ -1668,23 +1737,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">locationRemarks
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+          <t xml:space="preserve">vUTM
+</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -1710,223 +1767,183 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Use this column to denote information about plot location or polygon number, or miscellaneous notes that discuss the relative position or the state of the habitat/ site
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: poly 20
-</t>
+          <t xml:space="preserve">if verbatim coordinates in UTM, denote in this column. Separate into 3 strings. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10U 45689 55678</t>
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{9F8D95FB-54D3-F04C-9134-F2DD1CEAD6ED}">
+    <comment ref="T1" authorId="1" shapeId="0" xr:uid="{C36EAF92-CB2B-8247-A6B4-E6839E892AD6}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">vLat 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Definition:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> verbatim latitude. The geographic latitude in decimal degrees or degrees minutes seconds. Positive values are north of the Equator, negative values are south of it. Legal values lie between -90 and 90, inclusive.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Examples: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> "-41.0983423". If degrees minutes seconds: 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>49 39 12</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vCoordUncertainty
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">denote the verbatim coordinate uncertainty in meters if provided with associated verbatim UTM or degree coordinates 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">30 </t>
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{A76DD89C-13AB-F048-A935-8FD1A912F16A}">
+    <comment ref="U1" authorId="1" shapeId="0" xr:uid="{A2F25764-4BE8-0245-85D4-5F505ECE445E}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">RECOMMENDED
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Definition:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">verbatim longitude. The geographic longitude in decimal degrees or degrees minutes seconds. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Positive values are east of the Greenwich Meridian, negative values are west of it. Legal values lie between -180 and 180, inclusive.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Examples: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> "-121.1761111". If in degrees minutes secons: 124 56 37</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">habitat 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Defintion: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>if habitat information provided, place here. This includes whether it is in an aquatic vs terrestrial habitat (aquatic, in lake shoreline), the biogeoclimatic zone, shading conditions (e.g. in shade, shaded, in sun) , relative position at locality (e.g. base vs seep vs ledge), position on habitat objects (e.g. on log)</t>
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="1" shapeId="0" xr:uid="{B3BFE285-5D7E-014B-96D5-A3177370E856}">
+    <comment ref="V1" authorId="1" shapeId="0" xr:uid="{1762D171-209D-D947-8555-AFF34FF14DD2}">
       <text>
         <r>
           <rPr>
@@ -1936,11 +1953,23 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">vUTM
-</t>
-        </r>
-        <r>
-          <rPr>
+          <t xml:space="preserve">assTaxa
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -1966,7 +1995,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">if verbatim coordinates in UTM, denote in this column. Separate into 3 strings. 
+          <t xml:space="preserve">associated taxa. Use this field to denote scientific names of associated taxa. HOWEVER, only do this if that associated taxa has a collection number/ is a collected specimen. Otherwise leave blank. 
 </t>
         </r>
         <r>
@@ -1996,26 +2025,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>10U 45689 55678</t>
+          <t>Isoetes echinospora</t>
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1" shapeId="0" xr:uid="{C36EAF92-CB2B-8247-A6B4-E6839E892AD6}">
+    <comment ref="W1" authorId="1" shapeId="0" xr:uid="{C6473173-DDA5-D44D-87A7-A892FDDB11D3}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">vCoordUncertainty
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">assOcc
+</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -2041,7 +2068,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">denote the verbatim coordinate uncertainty in meters if provided with associated verbatim UTM or degree coordinates 
+          <t xml:space="preserve">the occurrence numbers of taxa growing with this occurrence. HOWEVER, when entering data, only input data in this column if occurrence was growing with a specimen that was collected. Record the collection number here with HJC to indicate collected specimen
 </t>
         </r>
         <r>
@@ -2071,7 +2098,85 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">30 </t>
+          <t>"HJC-2863"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="1" shapeId="0" xr:uid="{B9586400-66D1-7141-8F4F-DF928AA236E2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">locationRemarks
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Use this column to denote information about plot location or polygon number, or miscellaneous notes that discuss the relative position or the state of the habitat/ site
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: poly 20
+</t>
         </r>
       </text>
     </comment>
@@ -2345,166 +2450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="1" shapeId="0" xr:uid="{C6473173-DDA5-D44D-87A7-A892FDDB11D3}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">assOcc
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">the occurrence numbers of taxa growing with this occurrence. HOWEVER, when entering data, only input data in this column if occurrence was growing with a specimen that was collected. Record the collection number here with HJC to indicate collected specimen
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>"HJC-2863"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AG1" authorId="1" shapeId="0" xr:uid="{1762D171-209D-D947-8555-AFF34FF14DD2}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">assTaxa
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">associated taxa. Use this field to denote scientific names of associated taxa. HOWEVER, only do this if that associated taxa has a collection number/ is a collected specimen. Otherwise leave blank. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Isoetes echinospora</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AH1" authorId="1" shapeId="0" xr:uid="{C09B578E-7BE1-1A44-890C-B5193E01F5A0}">
+    <comment ref="AF1" authorId="1" shapeId="0" xr:uid="{C09B578E-7BE1-1A44-890C-B5193E01F5A0}">
       <text>
         <r>
           <rPr>
@@ -2595,14 +2541,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>habitat</t>
   </si>
   <si>
-    <t>islandGroup</t>
-  </si>
-  <si>
     <t>island</t>
   </si>
   <si>
@@ -2693,9 +2636,6 @@
     <t>phenology</t>
   </si>
   <si>
-    <t>vElevRef</t>
-  </si>
-  <si>
     <t>vElevM</t>
   </si>
   <si>
@@ -2703,9 +2643,6 @@
   </si>
   <si>
     <t>h</t>
-  </si>
-  <si>
-    <t>species</t>
   </si>
   <si>
     <t>Canada</t>
@@ -3194,12 +3131,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
-  <dimension ref="A1:AH64"/>
+  <dimension ref="A1:AF64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3211,140 +3148,133 @@
     <col min="5" max="5" width="24.83203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="4" customWidth="1"/>
     <col min="7" max="7" width="24.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="4" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" style="4"/>
-    <col min="10" max="10" width="14.33203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="4" customWidth="1"/>
     <col min="11" max="11" width="26" style="4" customWidth="1"/>
     <col min="12" max="12" width="9" style="4" customWidth="1"/>
     <col min="13" max="13" width="16.83203125" style="4" customWidth="1"/>
     <col min="14" max="14" width="20.33203125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="21.5" style="4" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="22.1640625" style="4" customWidth="1"/>
-    <col min="18" max="19" width="8.5" style="4" customWidth="1"/>
-    <col min="20" max="20" width="16.83203125" style="4" customWidth="1"/>
-    <col min="21" max="21" width="9.1640625" style="4" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="19.1640625" style="4" customWidth="1"/>
-    <col min="24" max="24" width="11.33203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="8.5" style="4" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" style="4" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" style="4" customWidth="1"/>
+    <col min="21" max="21" width="22.1640625" style="4" customWidth="1"/>
+    <col min="22" max="22" width="29.5" style="4" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="16.83203125" style="4" customWidth="1"/>
     <col min="25" max="25" width="7.5" style="4" customWidth="1"/>
     <col min="26" max="26" width="11.33203125" style="4" customWidth="1"/>
     <col min="27" max="27" width="11.1640625" style="4" customWidth="1"/>
     <col min="28" max="28" width="13" style="4" customWidth="1"/>
-    <col min="29" max="29" width="9.1640625" style="4" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="7.1640625" style="4" customWidth="1"/>
+    <col min="30" max="30" width="9" style="4" customWidth="1"/>
     <col min="31" max="31" width="10.83203125" style="4"/>
-    <col min="32" max="32" width="14.33203125" style="4" customWidth="1"/>
-    <col min="33" max="33" width="29.5" style="4" customWidth="1"/>
-    <col min="34" max="34" width="70.6640625" style="4" customWidth="1"/>
-    <col min="35" max="16384" width="10.83203125" style="4"/>
+    <col min="32" max="32" width="70.6640625" style="4" customWidth="1"/>
+    <col min="33" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>7</v>
       </c>
@@ -3355,50 +3285,44 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J2" s="4">
         <v>19810528</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="W2"/>
-      <c r="X2"/>
-      <c r="AG2"/>
-      <c r="AH2"/>
-    </row>
-    <row r="3" spans="1:34" ht="17" x14ac:dyDescent="0.2">
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2"/>
+      <c r="AF2"/>
+    </row>
+    <row r="3" spans="1:32" ht="17" x14ac:dyDescent="0.2">
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
@@ -3406,13 +3330,13 @@
       <c r="F3"/>
       <c r="G3"/>
       <c r="K3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="AH3"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="AF3"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
@@ -3420,25 +3344,25 @@
       <c r="F4"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
-      <c r="AH5"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF5"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B6"/>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
-      <c r="AH6"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF6"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -3446,256 +3370,256 @@
       <c r="F7"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8"/>
-      <c r="AH8"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF8"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
-      <c r="AH9"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF9"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
-      <c r="AH10"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF10"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
-      <c r="Q11"/>
-      <c r="T11"/>
-      <c r="AH11"/>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="U11"/>
+      <c r="X11"/>
+      <c r="AF11"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
-      <c r="AH12"/>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF12"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="Q13"/>
-      <c r="T13"/>
+      <c r="U13"/>
+      <c r="X13"/>
       <c r="AB13"/>
       <c r="AC13"/>
-      <c r="AH13"/>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF13"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="Q14"/>
-      <c r="T14"/>
-      <c r="AH14"/>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="U14"/>
+      <c r="X14"/>
+      <c r="AF14"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="Q15"/>
-      <c r="T15"/>
-      <c r="AH15"/>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="U15"/>
+      <c r="X15"/>
+      <c r="AF15"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
-      <c r="Q16"/>
-      <c r="T16"/>
-      <c r="AH16"/>
-    </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U16"/>
+      <c r="X16"/>
+      <c r="AF16"/>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="Q17"/>
-      <c r="T17"/>
-      <c r="AH17"/>
-    </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U17"/>
+      <c r="X17"/>
+      <c r="AF17"/>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18"/>
-      <c r="Q18"/>
-      <c r="T18"/>
-      <c r="AH18"/>
-    </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U18"/>
+      <c r="X18"/>
+      <c r="AF18"/>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
-      <c r="Q19"/>
-      <c r="T19"/>
-      <c r="AH19"/>
-    </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U19"/>
+      <c r="X19"/>
+      <c r="AF19"/>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20"/>
-      <c r="Q20"/>
-      <c r="T20"/>
-      <c r="AH20"/>
-    </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U20"/>
+      <c r="X20"/>
+      <c r="AF20"/>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
-      <c r="Q21"/>
-      <c r="T21"/>
-      <c r="AH21"/>
-    </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U21"/>
+      <c r="X21"/>
+      <c r="AF21"/>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
-      <c r="Q22"/>
-      <c r="T22"/>
-      <c r="AH22"/>
-    </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U22"/>
+      <c r="X22"/>
+      <c r="AF22"/>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23"/>
-      <c r="Q23"/>
-      <c r="T23"/>
-      <c r="AH23"/>
-    </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U23"/>
+      <c r="X23"/>
+      <c r="AF23"/>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24"/>
-      <c r="Q24"/>
-      <c r="T24"/>
-      <c r="AH24"/>
-    </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U24"/>
+      <c r="X24"/>
+      <c r="AF24"/>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25"/>
-      <c r="Q25"/>
-      <c r="T25"/>
-      <c r="AH25"/>
-    </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U25"/>
+      <c r="X25"/>
+      <c r="AF25"/>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
-      <c r="Q26"/>
-      <c r="T26"/>
-      <c r="AH26"/>
-    </row>
-    <row r="27" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="U26"/>
+      <c r="X26"/>
+      <c r="AF26"/>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="T27"/>
-      <c r="AH27"/>
-    </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="X27"/>
+      <c r="AF27"/>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
-      <c r="AH28"/>
-    </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AF28"/>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="AH29"/>
-    </row>
-    <row r="30" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AF29"/>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
-      <c r="AH30"/>
-    </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AF30"/>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="AH31"/>
-    </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AF31"/>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B32"/>
       <c r="C32"/>
     </row>

</xml_diff>